<commit_message>
filtering by hour and month at the same time
</commit_message>
<xml_diff>
--- a/data/esc_a.xlsx
+++ b/data/esc_a.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Escritorio\proyecciones_eolicas\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72766516-1734-44B0-AEDD-C29CCD6290FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -31,12 +37,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-MMMM"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mmmm"/>
     <numFmt numFmtId="165" formatCode="#.0#############E+###"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +111,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -151,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,9 +197,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,6 +249,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,19 +442,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -415,7 +465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44927</v>
       </c>
@@ -423,10 +473,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>26.5709408602151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>26.570940860215099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44958</v>
       </c>
@@ -437,7 +487,7 @@
         <v>32.7697619047619</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44986</v>
       </c>
@@ -445,10 +495,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>42.9853494623656</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>42.985349462365598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45017</v>
       </c>
@@ -456,10 +506,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>41.3576527777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>41.357652777777801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45047</v>
       </c>
@@ -470,7 +520,7 @@
         <v>42.1421505376344</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45078</v>
       </c>
@@ -481,7 +531,7 @@
         <v>37.6463055555555</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45108</v>
       </c>
@@ -489,10 +539,10 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>36.7597446236559</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>36.759744623655898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45139</v>
       </c>
@@ -500,10 +550,10 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>32.9790860215054</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>32.979086021505402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45170</v>
       </c>
@@ -514,7 +564,7 @@
         <v>27.9267222222222</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45200</v>
       </c>
@@ -522,10 +572,10 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>24.5252956989247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>24.525295698924701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45231</v>
       </c>
@@ -533,10 +583,10 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>22.7325</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>22.732500000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45261</v>
       </c>
@@ -547,7 +597,7 @@
         <v>22.6848252688172</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45292</v>
       </c>
@@ -555,10 +605,10 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>28.71134408602152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>28.711344086021519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45323</v>
       </c>
@@ -566,10 +616,10 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>49.12142241379311</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>49.121422413793113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45352</v>
       </c>
@@ -577,10 +627,10 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>96.42489247311829</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>96.424892473118291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45383</v>
       </c>
@@ -588,10 +638,10 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>85.0871388888888</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>85.087138888888802</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45413</v>
       </c>
@@ -599,10 +649,10 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>85.25581989247311</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>85.255819892473113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45444</v>
       </c>
@@ -610,10 +660,10 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>70.727125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>70.727125000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45474</v>
       </c>
@@ -621,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>72.0095833333333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>72.009583333333296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45505</v>
       </c>
@@ -632,10 +682,10 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>58.4805107526882</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>58.480510752688197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45536</v>
       </c>
@@ -643,10 +693,10 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>46.9656805555555</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>46.965680555555501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45566</v>
       </c>
@@ -654,10 +704,10 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>39.2014919354839</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>39.201491935483901</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45597</v>
       </c>
@@ -668,7 +718,7 @@
         <v>33.8559861111111</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45627</v>
       </c>
@@ -676,10 +726,10 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>28.75114247311828</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>28.751142473118279</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45658</v>
       </c>
@@ -690,7 +740,7 @@
         <v>26.40932795698928</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45689</v>
       </c>
@@ -698,10 +748,10 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>38.88976190476195</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>38.889761904761947</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45717</v>
       </c>
@@ -709,10 +759,10 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>84.3086693548388</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>84.308669354838798</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45748</v>
       </c>
@@ -720,10 +770,10 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>77.15322222222221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>77.153222222222212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45778</v>
       </c>
@@ -731,10 +781,10 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>77.3696774193548</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>77.369677419354801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45809</v>
       </c>
@@ -742,10 +792,10 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>64.4180555555556</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>64.418055555555597</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45839</v>
       </c>
@@ -753,10 +803,10 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>63.6691532258065</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>63.669153225806497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45870</v>
       </c>
@@ -764,10 +814,10 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>48.1197983870967</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>48.119798387096701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45901</v>
       </c>
@@ -775,10 +825,10 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>35.98069444444448</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>35.980694444444481</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45931</v>
       </c>
@@ -789,7 +839,7 @@
         <v>28.3740456989247</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45962</v>
       </c>
@@ -797,10 +847,10 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <v>22.9958333333333</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>22.995833333333302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45992</v>
       </c>
@@ -808,10 +858,10 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>25.70260752688175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>25.702607526881749</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>46023</v>
       </c>
@@ -819,10 +869,10 @@
         <v>3</v>
       </c>
       <c r="C38">
-        <v>29.21688172043009</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>29.216881720430091</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>46054</v>
       </c>
@@ -830,10 +880,10 @@
         <v>3</v>
       </c>
       <c r="C39">
-        <v>45.53178571428573</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>45.531785714285732</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>46082</v>
       </c>
@@ -841,10 +891,10 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>94.55252688172041</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>94.552526881720411</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>46113</v>
       </c>
@@ -852,10 +902,10 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>84.68836111111111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>84.688361111111107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>46143</v>
       </c>
@@ -866,7 +916,7 @@
         <v>81.84216397849471</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>46174</v>
       </c>
@@ -874,10 +924,10 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>71.78940277777781</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>71.789402777777809</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>46204</v>
       </c>
@@ -885,10 +935,10 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>72.75345430107521</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>72.753454301075209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>46235</v>
       </c>
@@ -896,10 +946,10 @@
         <v>3</v>
       </c>
       <c r="C45">
-        <v>57.8709946236559</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>57.870994623655903</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>46266</v>
       </c>
@@ -907,10 +957,10 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>47.1416666666666</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>47.141666666666602</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46296</v>
       </c>
@@ -918,10 +968,10 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>39.46025537634405</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>39.460255376344051</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46327</v>
       </c>
@@ -929,10 +979,10 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>32.07773611111114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>32.077736111111143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>46357</v>
       </c>
@@ -940,10 +990,10 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>31.36975806451617</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>31.369758064516169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>46388</v>
       </c>
@@ -951,10 +1001,10 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>32.51741935483867</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>32.517419354838673</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>46419</v>
       </c>
@@ -962,10 +1012,10 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>49.14184523809523</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>49.141845238095229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>46447</v>
       </c>
@@ -976,7 +1026,7 @@
         <v>102.0389112903226</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>46478</v>
       </c>
@@ -984,10 +1034,10 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>92.8495555555555</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>92.849555555555497</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>46508</v>
       </c>
@@ -995,10 +1045,10 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>88.8602553763441</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>88.860255376344099</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>46539</v>
       </c>
@@ -1006,10 +1056,10 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>77.30705555555561</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>77.307055555555607</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>46569</v>
       </c>
@@ -1017,10 +1067,10 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>79.79866935483869</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>79.798669354838694</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>46600</v>
       </c>
@@ -1028,10 +1078,10 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>63.4744220430108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>63.474422043010797</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>46631</v>
       </c>
@@ -1042,7 +1092,7 @@
         <v>51.5391388888889</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>46661</v>
       </c>
@@ -1050,10 +1100,10 @@
         <v>3</v>
       </c>
       <c r="C59">
-        <v>42.37677419354842</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>42.376774193548421</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>46692</v>
       </c>
@@ -1061,10 +1111,10 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>35.3221527777778</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>35.322152777777802</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>46722</v>
       </c>
@@ -1072,10 +1122,10 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <v>34.39112903225809</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>34.391129032258092</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>46753</v>
       </c>
@@ -1083,10 +1133,10 @@
         <v>3</v>
       </c>
       <c r="C62">
-        <v>33.1161559139785</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>33.116155913978503</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>46784</v>
       </c>
@@ -1097,7 +1147,7 @@
         <v>51.40817528735635</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>46813</v>
       </c>
@@ -1108,7 +1158,7 @@
         <v>105.880752688172</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>46844</v>
       </c>
@@ -1116,10 +1166,10 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>92.03780555555559</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>92.037805555555593</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>46874</v>
       </c>
@@ -1127,10 +1177,10 @@
         <v>3</v>
       </c>
       <c r="C66">
-        <v>86.9459677419355</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>86.945967741935505</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>46905</v>
       </c>
@@ -1138,10 +1188,10 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>75.50125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>75.501249999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>46935</v>
       </c>
@@ -1149,10 +1199,10 @@
         <v>3</v>
       </c>
       <c r="C68">
-        <v>76.1452822580645</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>76.145282258064498</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>46966</v>
       </c>
@@ -1160,10 +1210,10 @@
         <v>3</v>
       </c>
       <c r="C69">
-        <v>59.9311021505377</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>59.931102150537697</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>46997</v>
       </c>
@@ -1171,10 +1221,10 @@
         <v>3</v>
       </c>
       <c r="C70">
-        <v>50.2018055555556</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>50.201805555555602</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>47027</v>
       </c>
@@ -1182,10 +1232,10 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <v>43.6971102150537</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>43.697110215053698</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>47058</v>
       </c>
@@ -1193,10 +1243,10 @@
         <v>3</v>
       </c>
       <c r="C72">
-        <v>37.24908333333337</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>37.249083333333367</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>47088</v>
       </c>
@@ -1204,10 +1254,10 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>34.54698924731183</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>34.546989247311828</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>47119</v>
       </c>
@@ -1215,10 +1265,10 @@
         <v>3</v>
       </c>
       <c r="C74">
-        <v>30.71297043010758</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>30.712970430107578</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>47150</v>
       </c>
@@ -1226,10 +1276,10 @@
         <v>3</v>
       </c>
       <c r="C75">
-        <v>50.48488095238091</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>50.484880952380912</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>47178</v>
       </c>
@@ -1240,7 +1290,7 @@
         <v>112.2533064516129</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>47209</v>
       </c>
@@ -1251,7 +1301,7 @@
         <v>102.1469583333333</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>47239</v>
       </c>
@@ -1262,7 +1312,7 @@
         <v>95.5614784946236</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>47270</v>
       </c>
@@ -1270,10 +1320,10 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>87.4327222222222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>87.432722222222196</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>47300</v>
       </c>
@@ -1281,10 +1331,10 @@
         <v>3</v>
       </c>
       <c r="C80">
-        <v>80.7952553763441</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>80.795255376344102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>47331</v>
       </c>
@@ -1292,10 +1342,10 @@
         <v>3</v>
       </c>
       <c r="C81">
-        <v>63.2548924731183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>63.254892473118304</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>47362</v>
       </c>
@@ -1303,10 +1353,10 @@
         <v>3</v>
       </c>
       <c r="C82">
-        <v>50.4600138888889</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>50.460013888888902</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>47392</v>
       </c>
@@ -1314,10 +1364,10 @@
         <v>3</v>
       </c>
       <c r="C83">
-        <v>48.1093951612903</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>48.109395161290301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>47423</v>
       </c>
@@ -1328,7 +1378,7 @@
         <v>34.17986111111113</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>47453</v>
       </c>
@@ -1336,10 +1386,10 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>34.41459677419358</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <v>34.414596774193583</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>47484</v>
       </c>
@@ -1347,10 +1397,10 @@
         <v>3</v>
       </c>
       <c r="C86">
-        <v>33.63034946236559</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <v>33.630349462365587</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>47515</v>
       </c>
@@ -1358,10 +1408,10 @@
         <v>3</v>
       </c>
       <c r="C87">
-        <v>50.55172619047622</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>50.551726190476217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>47543</v>
       </c>
@@ -1372,7 +1422,7 @@
         <v>117.4654301075269</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>47574</v>
       </c>
@@ -1380,10 +1430,10 @@
         <v>3</v>
       </c>
       <c r="C89">
-        <v>105.1482777777778</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <v>105.14827777777781</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>47604</v>
       </c>
@@ -1394,7 +1444,7 @@
         <v>94.8084274193548</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>47635</v>
       </c>
@@ -1402,10 +1452,10 @@
         <v>3</v>
       </c>
       <c r="C91">
-        <v>80.9122361111111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <v>80.912236111111099</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>47665</v>
       </c>
@@ -1413,10 +1463,10 @@
         <v>3</v>
       </c>
       <c r="C92">
-        <v>74.48439516129031</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>74.484395161290308</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>47696</v>
       </c>
@@ -1424,10 +1474,10 @@
         <v>3</v>
       </c>
       <c r="C93">
-        <v>52.2354166666666</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>52.235416666666602</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>47727</v>
       </c>
@@ -1435,10 +1485,10 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>46.8251805555556</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>46.825180555555598</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>47757</v>
       </c>
@@ -1446,10 +1496,10 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>44.6333333333334</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+        <v>44.633333333333397</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>47788</v>
       </c>
@@ -1460,7 +1510,7 @@
         <v>32.24004166666667</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>47818</v>
       </c>
@@ -1471,7 +1521,7 @@
         <v>31.40958333333333</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>47849</v>
       </c>
@@ -1479,10 +1529,10 @@
         <v>3</v>
       </c>
       <c r="C98">
-        <v>35.74505376344086</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>35.745053763440858</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>47880</v>
       </c>
@@ -1490,10 +1540,10 @@
         <v>3</v>
       </c>
       <c r="C99">
-        <v>55.2295833333333</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+        <v>55.229583333333302</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>47908</v>
       </c>
@@ -1501,10 +1551,10 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>124.8139112903226</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+        <v>124.81391129032259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>47939</v>
       </c>
@@ -1515,7 +1565,7 @@
         <v>108.7020555555555</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>47969</v>
       </c>
@@ -1523,10 +1573,10 @@
         <v>3</v>
       </c>
       <c r="C102">
-        <v>99.59275537634412</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <v>99.592755376344115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>48000</v>
       </c>
@@ -1534,10 +1584,10 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>84.95762500000001</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>84.957625000000007</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>48030</v>
       </c>
@@ -1545,10 +1595,10 @@
         <v>3</v>
       </c>
       <c r="C104">
-        <v>76.5500672043011</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <v>76.550067204301101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>48061</v>
       </c>
@@ -1556,10 +1606,10 @@
         <v>3</v>
       </c>
       <c r="C105">
-        <v>55.624932795699</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>55.624932795699003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>48092</v>
       </c>
@@ -1567,10 +1617,10 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>51.8250972222222</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>51.825097222222198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>48122</v>
       </c>
@@ -1578,10 +1628,10 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>46.8079569892473</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>46.807956989247302</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>48153</v>
       </c>
@@ -1589,10 +1639,10 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>34.42206944444442</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>34.422069444444418</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>48183</v>
       </c>
@@ -1600,10 +1650,10 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>34.54927419354835</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>34.549274193548349</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>48214</v>
       </c>
@@ -1611,10 +1661,10 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>34.41633064516124</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>34.416330645161239</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>48245</v>
       </c>
@@ -1622,10 +1672,10 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>55.05413793103446</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <v>55.054137931034461</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>48274</v>
       </c>
@@ -1633,10 +1683,10 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>132.9367741935484</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
+        <v>132.93677419354839</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>48305</v>
       </c>
@@ -1647,7 +1697,7 @@
         <v>114.6786111111111</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>48335</v>
       </c>
@@ -1658,7 +1708,7 @@
         <v>100.9956048387097</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>48366</v>
       </c>
@@ -1666,10 +1716,10 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>88.22641666666669</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
+        <v>88.226416666666694</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>48396</v>
       </c>
@@ -1677,10 +1727,10 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>82.9170967741936</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+        <v>82.917096774193595</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>48427</v>
       </c>
@@ -1688,10 +1738,10 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>61.1316801075269</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
+        <v>61.131680107526897</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>48458</v>
       </c>
@@ -1699,10 +1749,10 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>51.2568333333334</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
+        <v>51.256833333333397</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>48488</v>
       </c>
@@ -1710,10 +1760,10 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>49.0250672043011</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+        <v>49.025067204301102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>48519</v>
       </c>
@@ -1721,10 +1771,10 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>33.11993055555558</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
+        <v>33.119930555555577</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>48549</v>
       </c>
@@ -1732,10 +1782,10 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>33.71611559139784</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
+        <v>33.716115591397838</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>48580</v>
       </c>
@@ -1743,10 +1793,10 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>39.14063172043008</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
+        <v>39.140631720430079</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>48611</v>
       </c>
@@ -1754,10 +1804,10 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>58.55636904761902</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
+        <v>58.556369047619022</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>48639</v>
       </c>
@@ -1768,7 +1818,7 @@
         <v>141.9174865591398</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>48670</v>
       </c>
@@ -1779,7 +1829,7 @@
         <v>120.5885972222223</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>48700</v>
       </c>
@@ -1787,10 +1837,10 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>108.2859139784946</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
+        <v>108.28591397849461</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>48731</v>
       </c>
@@ -1798,10 +1848,10 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>94.3198055555556</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
+        <v>94.319805555555604</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>48761</v>
       </c>
@@ -1809,10 +1859,10 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>86.04561827956991</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
+        <v>86.045618279569908</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>48792</v>
       </c>
@@ -1820,10 +1870,10 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>64.8705107526882</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
+        <v>64.870510752688205</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>48823</v>
       </c>
@@ -1831,10 +1881,10 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>57.98294444444441</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+        <v>57.982944444444414</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>48853</v>
       </c>
@@ -1842,10 +1892,10 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>49.8278897849462</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+        <v>49.827889784946201</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>48884</v>
       </c>
@@ -1853,10 +1903,10 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>36.19002777777781</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
+        <v>36.190027777777807</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>48914</v>
       </c>
@@ -1864,10 +1914,10 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>35.50748655913978</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+        <v>35.507486559139778</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>48945</v>
       </c>
@@ -1875,10 +1925,10 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>36.22119623655914</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+        <v>36.221196236559138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>48976</v>
       </c>
@@ -1886,10 +1936,10 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>54.16750000000002</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
+        <v>54.167500000000018</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>49004</v>
       </c>
@@ -1900,7 +1950,7 @@
         <v>126.4491801075268</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>49035</v>
       </c>
@@ -1911,7 +1961,7 @@
         <v>110.54525</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>49065</v>
       </c>
@@ -1919,10 +1969,10 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>96.1275</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+        <v>96.127499999999998</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>49096</v>
       </c>
@@ -1930,10 +1980,10 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>86.1462777777778</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+        <v>86.146277777777797</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>49126</v>
       </c>
@@ -1941,10 +1991,10 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>76.99920698924731</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
+        <v>76.999206989247313</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>49157</v>
       </c>
@@ -1952,10 +2002,10 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>55.34950268817209</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+        <v>55.349502688172088</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>49188</v>
       </c>
@@ -1963,10 +2013,10 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>48.3903055555556</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
+        <v>48.390305555555599</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>49218</v>
       </c>
@@ -1974,10 +2024,10 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>44.4274193548388</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+        <v>44.427419354838797</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>49249</v>
       </c>
@@ -1988,7 +2038,7 @@
         <v>31.64869444444442</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>49279</v>
       </c>
@@ -1996,10 +2046,10 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>30.62005376344083</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
+        <v>30.620053763440829</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>49310</v>
       </c>
@@ -2007,10 +2057,10 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>35.10493279569889</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
+        <v>35.104932795698893</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>49341</v>
       </c>
@@ -2018,10 +2068,10 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>59.95255952380958</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
+        <v>59.952559523809583</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>49369</v>
       </c>
@@ -2029,10 +2079,10 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>138.3921908602151</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
+        <v>138.39219086021509</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>49400</v>
       </c>
@@ -2040,10 +2090,10 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>117.2619305555555</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
+        <v>117.26193055555549</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>49430</v>
       </c>
@@ -2051,10 +2101,10 @@
         <v>3</v>
       </c>
       <c r="C150">
-        <v>105.4752150537634</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
+        <v>105.47521505376341</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>49461</v>
       </c>
@@ -2062,10 +2112,10 @@
         <v>3</v>
       </c>
       <c r="C151">
-        <v>99.22970833333341</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
+        <v>99.229708333333406</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>49491</v>
       </c>
@@ -2073,10 +2123,10 @@
         <v>3</v>
       </c>
       <c r="C152">
-        <v>89.381559139785</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
+        <v>89.381559139784997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>49522</v>
       </c>
@@ -2087,7 +2137,7 @@
         <v>62.2296774193548</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>49553</v>
       </c>
@@ -2095,10 +2145,10 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>49.9106944444445</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
+        <v>49.910694444444502</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>49583</v>
       </c>
@@ -2106,10 +2156,10 @@
         <v>3</v>
       </c>
       <c r="C155">
-        <v>42.56723118279574</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
+        <v>42.567231182795737</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>49614</v>
       </c>
@@ -2120,7 +2170,7 @@
         <v>30.79413888888892</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>49644</v>
       </c>
@@ -2131,7 +2181,7 @@
         <v>31.6466666666667</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>49675</v>
       </c>
@@ -2139,10 +2189,10 @@
         <v>3</v>
       </c>
       <c r="C158">
-        <v>38.69994623655916</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
+        <v>38.699946236559157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>49706</v>
       </c>
@@ -2150,10 +2200,10 @@
         <v>3</v>
       </c>
       <c r="C159">
-        <v>64.37405172413794</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
+        <v>64.374051724137942</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>49735</v>
       </c>
@@ -2161,10 +2211,10 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>142.994193548387</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+        <v>142.99419354838699</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>49766</v>
       </c>
@@ -2175,7 +2225,7 @@
         <v>119.3128055555556</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>49796</v>
       </c>
@@ -2186,7 +2236,7 @@
         <v>114.6330913978495</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>49827</v>
       </c>
@@ -2194,10 +2244,10 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>106.6436805555555</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
+        <v>106.64368055555551</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>49857</v>
       </c>
@@ -2205,10 +2255,10 @@
         <v>3</v>
       </c>
       <c r="C164">
-        <v>100.2427688172043</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+        <v>100.24276881720429</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>49888</v>
       </c>
@@ -2216,10 +2266,10 @@
         <v>3</v>
       </c>
       <c r="C165">
-        <v>67.9263440860215</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>67.926344086021501</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>49919</v>
       </c>
@@ -2227,10 +2277,10 @@
         <v>3</v>
       </c>
       <c r="C166">
-        <v>56.57825</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
+        <v>56.578249999999997</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>49949</v>
       </c>
@@ -2238,10 +2288,10 @@
         <v>3</v>
       </c>
       <c r="C167">
-        <v>44.9493279569892</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+        <v>44.949327956989201</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>49980</v>
       </c>
@@ -2249,10 +2299,10 @@
         <v>3</v>
       </c>
       <c r="C168">
-        <v>33.35516666666667</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
+        <v>33.355166666666669</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>50010</v>
       </c>
@@ -2260,10 +2310,10 @@
         <v>3</v>
       </c>
       <c r="C169">
-        <v>34.70626344086018</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
+        <v>34.706263440860177</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>50041</v>
       </c>
@@ -2271,10 +2321,10 @@
         <v>3</v>
       </c>
       <c r="C170">
-        <v>30.43435483870965</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
+        <v>30.434354838709648</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>50072</v>
       </c>
@@ -2282,10 +2332,10 @@
         <v>3</v>
       </c>
       <c r="C171">
-        <v>58.32232142857143</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
+        <v>58.322321428571428</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>50100</v>
       </c>
@@ -2293,10 +2343,10 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>137.6127419354839</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
+        <v>137.61274193548391</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>50131</v>
       </c>
@@ -2304,10 +2354,10 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>112.7991666666667</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
+        <v>112.79916666666669</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>50161</v>
       </c>
@@ -2315,10 +2365,10 @@
         <v>3</v>
       </c>
       <c r="C174">
-        <v>107.9147849462366</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+        <v>107.91478494623659</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>50192</v>
       </c>
@@ -2326,10 +2376,10 @@
         <v>3</v>
       </c>
       <c r="C175">
-        <v>98.9741527777778</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+        <v>98.974152777777803</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>50222</v>
       </c>
@@ -2337,10 +2387,10 @@
         <v>3</v>
       </c>
       <c r="C176">
-        <v>94.7424596774194</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
+        <v>94.742459677419404</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>50253</v>
       </c>
@@ -2348,10 +2398,10 @@
         <v>3</v>
       </c>
       <c r="C177">
-        <v>61.33823924731191</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
+        <v>61.338239247311911</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>50284</v>
       </c>
@@ -2359,10 +2409,10 @@
         <v>3</v>
       </c>
       <c r="C178">
-        <v>45.8660277777778</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
+        <v>45.866027777777802</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>50314</v>
       </c>
@@ -2370,10 +2420,10 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>37.931814516129</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
+        <v>37.931814516129002</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>50345</v>
       </c>
@@ -2381,10 +2431,10 @@
         <v>3</v>
       </c>
       <c r="C180">
-        <v>29.34454166666667</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
+        <v>29.344541666666672</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>50375</v>
       </c>
@@ -2392,10 +2442,10 @@
         <v>3</v>
       </c>
       <c r="C181">
-        <v>26.30970430107527</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
+        <v>26.309704301075271</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>50406</v>
       </c>
@@ -2403,10 +2453,10 @@
         <v>3</v>
       </c>
       <c r="C182">
-        <v>33.64448924731178</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
+        <v>33.644489247311782</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>50437</v>
       </c>
@@ -2417,7 +2467,7 @@
         <v>61.67791666666664</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>50465</v>
       </c>
@@ -2425,10 +2475,10 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>142.7499865591398</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+        <v>142.74998655913981</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>50496</v>
       </c>
@@ -2439,7 +2489,7 @@
         <v>119.5261944444444</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>50526</v>
       </c>
@@ -2450,7 +2500,7 @@
         <v>114.3686021505376</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>50557</v>
       </c>
@@ -2461,7 +2511,7 @@
         <v>104.4105</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>50587</v>
       </c>
@@ -2472,7 +2522,7 @@
         <v>101.1951075268818</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>50618</v>
       </c>
@@ -2480,10 +2530,10 @@
         <v>3</v>
       </c>
       <c r="C189">
-        <v>68.58825268817201</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
+        <v>68.588252688172005</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>50649</v>
       </c>
@@ -2494,7 +2544,7 @@
         <v>52.1625555555555</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>50679</v>
       </c>
@@ -2502,10 +2552,10 @@
         <v>3</v>
       </c>
       <c r="C191">
-        <v>44.6994623655914</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
+        <v>44.699462365591401</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>50710</v>
       </c>
@@ -2513,10 +2563,10 @@
         <v>3</v>
       </c>
       <c r="C192">
-        <v>33.08080555555552</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
+        <v>33.080805555555521</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>50740</v>
       </c>
@@ -2527,7 +2577,7 @@
         <v>33.12418010752684</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>50771</v>
       </c>
@@ -2538,7 +2588,7 @@
         <v>36.82716397849461</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>50802</v>
       </c>
@@ -2546,10 +2596,10 @@
         <v>3</v>
       </c>
       <c r="C195">
-        <v>66.71363095238098</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
+        <v>66.713630952380981</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>50830</v>
       </c>
@@ -2557,10 +2607,10 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>155.7927150537635</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
+        <v>155.79271505376349</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>50861</v>
       </c>
@@ -2571,7 +2621,7 @@
         <v>127.0055416666666</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>50891</v>
       </c>
@@ -2582,7 +2632,7 @@
         <v>121.4574865591397</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>50922</v>
       </c>
@@ -2590,10 +2640,10 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>116.3654722222222</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
+        <v>116.36547222222219</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>50952</v>
       </c>
@@ -2604,7 +2654,7 @@
         <v>114.6955510752688</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>50983</v>
       </c>
@@ -2615,7 +2665,7 @@
         <v>79.9461424731183</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>51014</v>
       </c>
@@ -2623,10 +2673,10 @@
         <v>3</v>
       </c>
       <c r="C202">
-        <v>63.52344444444451</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
+        <v>63.523444444444507</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>51044</v>
       </c>
@@ -2634,10 +2684,10 @@
         <v>3</v>
       </c>
       <c r="C203">
-        <v>49.8015053763441</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
+        <v>49.801505376344103</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>51075</v>
       </c>
@@ -2645,10 +2695,10 @@
         <v>3</v>
       </c>
       <c r="C204">
-        <v>37.27797222222218</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
+        <v>37.277972222222182</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>51105</v>
       </c>
@@ -2656,10 +2706,10 @@
         <v>3</v>
       </c>
       <c r="C205">
-        <v>36.19780913978495</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
+        <v>36.197809139784951</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>51136</v>
       </c>
@@ -2667,10 +2717,10 @@
         <v>3</v>
       </c>
       <c r="C206">
-        <v>39.56219086021501</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3">
+        <v>39.562190860215011</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>51167</v>
       </c>
@@ -2678,10 +2728,10 @@
         <v>3</v>
       </c>
       <c r="C207">
-        <v>69.21511494252874</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
+        <v>69.215114942528743</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>51196</v>
       </c>
@@ -2692,7 +2742,7 @@
         <v>161.3172177419352</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>51227</v>
       </c>
@@ -2703,7 +2753,7 @@
         <v>131.7024583333334</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>51257</v>
       </c>
@@ -2711,10 +2761,10 @@
         <v>3</v>
       </c>
       <c r="C210">
-        <v>124.5011693548387</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
+        <v>124.50116935483869</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>51288</v>
       </c>
@@ -2725,7 +2775,7 @@
         <v>124.1084722222223</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>51318</v>
       </c>
@@ -2736,7 +2786,7 @@
         <v>124.2471639784947</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>51349</v>
       </c>
@@ -2744,10 +2794,10 @@
         <v>3</v>
       </c>
       <c r="C213">
-        <v>87.28822580645161</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
+        <v>87.288225806451607</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>51380</v>
       </c>
@@ -2755,10 +2805,10 @@
         <v>3</v>
       </c>
       <c r="C214">
-        <v>66.5941111111111</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
+        <v>66.594111111111104</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>51410</v>
       </c>
@@ -2766,10 +2816,10 @@
         <v>3</v>
       </c>
       <c r="C215">
-        <v>50.4604838709678</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
+        <v>50.460483870967799</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>51441</v>
       </c>
@@ -2777,10 +2827,10 @@
         <v>3</v>
       </c>
       <c r="C216">
-        <v>38.18961111111109</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
+        <v>38.189611111111091</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>51471</v>
       </c>
@@ -2788,10 +2838,10 @@
         <v>3</v>
       </c>
       <c r="C217">
-        <v>39.15723118279565</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
+        <v>39.157231182795648</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>51502</v>
       </c>
@@ -2799,10 +2849,10 @@
         <v>3</v>
       </c>
       <c r="C218">
-        <v>43.02971774193547</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
+        <v>43.029717741935471</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>51533</v>
       </c>
@@ -2810,10 +2860,10 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>69.09708333333332</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
+        <v>69.097083333333316</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>51561</v>
       </c>
@@ -2821,10 +2871,10 @@
         <v>3</v>
       </c>
       <c r="C220">
-        <v>163.6395430107526</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
+        <v>163.63954301075259</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>51592</v>
       </c>
@@ -2835,7 +2885,7 @@
         <v>130.5584444444444</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>51622</v>
       </c>
@@ -2846,7 +2896,7 @@
         <v>125.0500940860215</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>51653</v>
       </c>
@@ -2854,10 +2904,10 @@
         <v>3</v>
       </c>
       <c r="C223">
-        <v>133.6494027777778</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
+        <v>133.64940277777779</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>51683</v>
       </c>
@@ -2868,7 +2918,7 @@
         <v>128.0794758064516</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>51714</v>
       </c>
@@ -2876,10 +2926,10 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>85.7774193548387</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
+        <v>85.777419354838699</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>51745</v>
       </c>
@@ -2887,10 +2937,10 @@
         <v>3</v>
       </c>
       <c r="C226">
-        <v>64.5315555555556</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
+        <v>64.531555555555599</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>51775</v>
       </c>
@@ -2898,10 +2948,10 @@
         <v>3</v>
       </c>
       <c r="C227">
-        <v>50.8413172043011</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
+        <v>50.841317204301099</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>51806</v>
       </c>
@@ -2912,7 +2962,7 @@
         <v>38.03744444444439</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>51836</v>
       </c>
@@ -2920,10 +2970,10 @@
         <v>3</v>
       </c>
       <c r="C229">
-        <v>43.38579301075267</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
+        <v>43.385793010752671</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>51867</v>
       </c>
@@ -2931,10 +2981,10 @@
         <v>3</v>
       </c>
       <c r="C230">
-        <v>45.99908602150539</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
+        <v>45.999086021505391</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>51898</v>
       </c>
@@ -2942,10 +2992,10 @@
         <v>3</v>
       </c>
       <c r="C231">
-        <v>70.9947619047619</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
+        <v>70.994761904761901</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>51926</v>
       </c>
@@ -2956,7 +3006,7 @@
         <v>171.2832526881725</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>51957</v>
       </c>
@@ -2964,10 +3014,10 @@
         <v>3</v>
       </c>
       <c r="C233">
-        <v>134.3465277777778</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
+        <v>134.34652777777779</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>51987</v>
       </c>
@@ -2975,10 +3025,10 @@
         <v>3</v>
       </c>
       <c r="C234">
-        <v>130.4417338709678</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
+        <v>130.44173387096779</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>52018</v>
       </c>
@@ -2986,10 +3036,10 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>137.5774861111111</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
+        <v>137.57748611111111</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>52048</v>
       </c>
@@ -2997,10 +3047,10 @@
         <v>3</v>
       </c>
       <c r="C236">
-        <v>132.1006586021506</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
+        <v>132.10065860215059</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>52079</v>
       </c>
@@ -3008,10 +3058,10 @@
         <v>3</v>
       </c>
       <c r="C237">
-        <v>88.02987903225811</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
+        <v>88.029879032258108</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>52110</v>
       </c>
@@ -3019,10 +3069,10 @@
         <v>3</v>
       </c>
       <c r="C238">
-        <v>67.94547222222219</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
+        <v>67.945472222222193</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>52140</v>
       </c>
@@ -3030,10 +3080,10 @@
         <v>3</v>
       </c>
       <c r="C239">
-        <v>52.9648387096774</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
+        <v>52.964838709677402</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>52171</v>
       </c>
@@ -3044,7 +3094,7 @@
         <v>39.0798611111111</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>52201</v>
       </c>
@@ -3052,10 +3102,10 @@
         <v>3</v>
       </c>
       <c r="C241">
-        <v>45.07803763440855</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
+        <v>45.078037634408552</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>52232</v>
       </c>
@@ -3066,7 +3116,7 @@
         <v>47.61795698924734</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>52263</v>
       </c>
@@ -3074,10 +3124,10 @@
         <v>3</v>
       </c>
       <c r="C243">
-        <v>73.8998809523809</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
+        <v>73.899880952380897</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>52291</v>
       </c>
@@ -3085,10 +3135,10 @@
         <v>3</v>
       </c>
       <c r="C244">
-        <v>170.8211021505379</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
+        <v>170.82110215053791</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>52322</v>
       </c>
@@ -3096,10 +3146,10 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>133.377</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
+        <v>133.37700000000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>52352</v>
       </c>
@@ -3107,10 +3157,10 @@
         <v>3</v>
       </c>
       <c r="C246">
-        <v>133.988938172043</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
+        <v>133.98893817204299</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>52383</v>
       </c>
@@ -3121,7 +3171,7 @@
         <v>137.0140277777777</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>52413</v>
       </c>
@@ -3129,10 +3179,10 @@
         <v>3</v>
       </c>
       <c r="C248">
-        <v>133.8992607526882</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
+        <v>133.89926075268821</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>52444</v>
       </c>
@@ -3140,10 +3190,10 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>93.19274193548391</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3">
+        <v>93.192741935483909</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>52475</v>
       </c>
@@ -3154,7 +3204,7 @@
         <v>71.52583333333331</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>52505</v>
       </c>
@@ -3162,10 +3212,10 @@
         <v>3</v>
       </c>
       <c r="C251">
-        <v>53.55145161290329</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
+        <v>53.551451612903293</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>52536</v>
       </c>
@@ -3173,10 +3223,10 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <v>39.26404166666664</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
+        <v>39.264041666666643</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>52566</v>
       </c>
@@ -3184,10 +3234,10 @@
         <v>3</v>
       </c>
       <c r="C253">
-        <v>51.1916666666667</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
+        <v>51.191666666666698</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>52597</v>
       </c>
@@ -3195,10 +3245,10 @@
         <v>3</v>
       </c>
       <c r="C254">
-        <v>51.99377688172044</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
+        <v>51.993776881720443</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>52628</v>
       </c>
@@ -3206,10 +3256,10 @@
         <v>3</v>
       </c>
       <c r="C255">
-        <v>72.27172413793109</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
+        <v>72.271724137931088</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>52657</v>
       </c>
@@ -3220,7 +3270,7 @@
         <v>192.4386693548384</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>52688</v>
       </c>
@@ -3231,7 +3281,7 @@
         <v>31.1523888888889</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>52718</v>
       </c>
@@ -3239,10 +3289,10 @@
         <v>3</v>
       </c>
       <c r="C258">
-        <v>33.5997580645161</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
+        <v>33.599758064516102</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>52749</v>
       </c>
@@ -3253,7 +3303,7 @@
         <v>28.4878055555556</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>52779</v>
       </c>
@@ -3261,10 +3311,10 @@
         <v>3</v>
       </c>
       <c r="C260">
-        <v>31.6575672043011</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
+        <v>31.657567204301099</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>52810</v>
       </c>
@@ -3272,10 +3322,10 @@
         <v>3</v>
       </c>
       <c r="C261">
-        <v>20.3714516129032</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
+        <v>20.371451612903201</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>52841</v>
       </c>
@@ -3286,7 +3336,7 @@
         <v>11.9196111111111</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>52871</v>
       </c>
@@ -3294,10 +3344,10 @@
         <v>3</v>
       </c>
       <c r="C263">
-        <v>8.2429435483871</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
+        <v>8.2429435483870996</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>52902</v>
       </c>
@@ -3305,10 +3355,10 @@
         <v>3</v>
       </c>
       <c r="C264">
-        <v>3.95922222222222</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
+        <v>3.9592222222222202</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>52932</v>
       </c>
@@ -3316,10 +3366,10 @@
         <v>3</v>
       </c>
       <c r="C265">
-        <v>5.00243279569892</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3">
+        <v>5.0024327956989199</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>52963</v>
       </c>
@@ -3330,7 +3380,7 @@
         <v>1.66629032258064</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>52994</v>
       </c>
@@ -3338,10 +3388,10 @@
         <v>3</v>
       </c>
       <c r="C267">
-        <v>6.77547619047619</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
+        <v>6.7754761904761898</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>53022</v>
       </c>
@@ -3349,7 +3399,7 @@
         <v>3</v>
       </c>
       <c r="C268">
-        <v>43.8299462365591</v>
+        <v>43.829946236559103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>